<commit_message>
added remainder of Auto.Deadline and Auto.Schedule tests
</commit_message>
<xml_diff>
--- a/FuncTestPlanAutoScheduler.xlsx
+++ b/FuncTestPlanAutoScheduler.xlsx
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="85" uniqueCount="51">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="93" uniqueCount="62">
   <si>
     <t>Test ID</t>
   </si>
@@ -177,6 +177,39 @@
   </si>
   <si>
     <t>Verifies AS does not move locked events</t>
+  </si>
+  <si>
+    <t>T_AS_S_3</t>
+  </si>
+  <si>
+    <t>Auto.Schedule.Location</t>
+  </si>
+  <si>
+    <t>Verifies AS schedules events within correct location events</t>
+  </si>
+  <si>
+    <t>2. Create a VS with location events for the same location as specified in the VD</t>
+  </si>
+  <si>
+    <t>1. Create a VD with a  location</t>
+  </si>
+  <si>
+    <t>2. Create an VS</t>
+  </si>
+  <si>
+    <t>Events with a specified location are contained within their a location event for the correct location.</t>
+  </si>
+  <si>
+    <t>Auto.Schedule.MoveEvent</t>
+  </si>
+  <si>
+    <t>Verifies AS can move non-locked, non-location events previously scheduled by the user.</t>
+  </si>
+  <si>
+    <t>Non-locked Events are moved to create space for AS's events so that they don't conflict with other events.</t>
+  </si>
+  <si>
+    <t>2. Create a VS with non-locked and locked events. Events within the VD's valid times must leave only just enough free time for deadline's total work time but not enough with the addition of breaks and max time constraints.</t>
   </si>
 </sst>
 </file>
@@ -530,10 +563,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:I37"/>
+  <dimension ref="A1:I41"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A14" workbookViewId="0">
-      <selection activeCell="G36" sqref="G36"/>
+    <sheetView tabSelected="1" topLeftCell="A24" workbookViewId="0">
+      <selection activeCell="D40" sqref="D40"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -834,7 +867,7 @@
       <c r="B23" s="4"/>
       <c r="C23" s="4"/>
       <c r="D23" s="2" t="s">
-        <v>15</v>
+        <v>56</v>
       </c>
       <c r="E23" s="4"/>
     </row>
@@ -946,27 +979,27 @@
     </row>
     <row r="34" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A34" s="4" t="s">
-        <v>45</v>
+        <v>51</v>
       </c>
       <c r="B34" s="4" t="s">
-        <v>46</v>
+        <v>52</v>
       </c>
       <c r="C34" s="4" t="s">
-        <v>50</v>
+        <v>53</v>
       </c>
       <c r="D34" s="2" t="s">
-        <v>14</v>
+        <v>55</v>
       </c>
       <c r="E34" s="4" t="s">
-        <v>49</v>
-      </c>
-    </row>
-    <row r="35" spans="1:5" x14ac:dyDescent="0.25">
+        <v>57</v>
+      </c>
+    </row>
+    <row r="35" spans="1:5" ht="30" x14ac:dyDescent="0.25">
       <c r="A35" s="4"/>
       <c r="B35" s="4"/>
       <c r="C35" s="4"/>
       <c r="D35" s="2" t="s">
-        <v>48</v>
+        <v>54</v>
       </c>
       <c r="E35" s="4"/>
     </row>
@@ -988,12 +1021,60 @@
       </c>
       <c r="E37" s="4"/>
     </row>
+    <row r="38" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A38" s="4" t="s">
+        <v>51</v>
+      </c>
+      <c r="B38" s="4" t="s">
+        <v>58</v>
+      </c>
+      <c r="C38" s="4" t="s">
+        <v>59</v>
+      </c>
+      <c r="D38" s="2" t="s">
+        <v>14</v>
+      </c>
+      <c r="E38" s="4" t="s">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="39" spans="1:5" ht="90" x14ac:dyDescent="0.25">
+      <c r="A39" s="4"/>
+      <c r="B39" s="4"/>
+      <c r="C39" s="4"/>
+      <c r="D39" s="2" t="s">
+        <v>61</v>
+      </c>
+      <c r="E39" s="4"/>
+    </row>
+    <row r="40" spans="1:5" ht="30" x14ac:dyDescent="0.25">
+      <c r="A40" s="4"/>
+      <c r="B40" s="4"/>
+      <c r="C40" s="4"/>
+      <c r="D40" s="2" t="s">
+        <v>16</v>
+      </c>
+      <c r="E40" s="4"/>
+    </row>
+    <row r="41" spans="1:5" ht="30" x14ac:dyDescent="0.25">
+      <c r="A41" s="4"/>
+      <c r="B41" s="4"/>
+      <c r="C41" s="4"/>
+      <c r="D41" s="2" t="s">
+        <v>17</v>
+      </c>
+      <c r="E41" s="4"/>
+    </row>
   </sheetData>
-  <mergeCells count="36">
+  <mergeCells count="40">
     <mergeCell ref="A34:A37"/>
     <mergeCell ref="B34:B37"/>
     <mergeCell ref="C34:C37"/>
     <mergeCell ref="E34:E37"/>
+    <mergeCell ref="A38:A41"/>
+    <mergeCell ref="B38:B41"/>
+    <mergeCell ref="C38:C41"/>
+    <mergeCell ref="E38:E41"/>
     <mergeCell ref="A26:A29"/>
     <mergeCell ref="B26:B29"/>
     <mergeCell ref="C26:C29"/>

</xml_diff>

<commit_message>
added Auto Scheduler diff tests to test plan
</commit_message>
<xml_diff>
--- a/FuncTestPlanAutoScheduler.xlsx
+++ b/FuncTestPlanAutoScheduler.xlsx
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="93" uniqueCount="62">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="141" uniqueCount="93">
   <si>
     <t>Test ID</t>
   </si>
@@ -143,6 +143,12 @@
     <t>Events have a period of time greater than or equal to deadline's time between before and after them.</t>
   </si>
   <si>
+    <t>Auto.Schedule</t>
+  </si>
+  <si>
+    <t>Auto.Schedule.Deadline</t>
+  </si>
+  <si>
     <t>Auto.Schedule.Conflicts</t>
   </si>
   <si>
@@ -210,6 +216,93 @@
   </si>
   <si>
     <t>2. Create a VS with non-locked and locked events. Events within the VD's valid times must leave only just enough free time for deadline's total work time but not enough with the addition of breaks and max time constraints.</t>
+  </si>
+  <si>
+    <t>T_AS_S_4</t>
+  </si>
+  <si>
+    <t>Auto.Diff</t>
+  </si>
+  <si>
+    <t>Auto.Deadline</t>
+  </si>
+  <si>
+    <t>T_AS_1</t>
+  </si>
+  <si>
+    <t>AS schedules events that don't conflict with currently in the VS and within the valid work times of the deadline.</t>
+  </si>
+  <si>
+    <t>T_Diff_1</t>
+  </si>
+  <si>
+    <t>Verify user is presented with graphical comparison of schedules after creating a deadline event</t>
+  </si>
+  <si>
+    <t>1. Open Event creation form</t>
+  </si>
+  <si>
+    <t>2. Select Deadline Event</t>
+  </si>
+  <si>
+    <t>3. Input valid deadline event parameters and submit</t>
+  </si>
+  <si>
+    <t>4. Graphical user interface comparing previous version of the schedule and schedule offered by AS given to user</t>
+  </si>
+  <si>
+    <t>User presented with graphical user interface to compare versions of schedules</t>
+  </si>
+  <si>
+    <t>T_Diff_2</t>
+  </si>
+  <si>
+    <t>Auto.Diff.Accept</t>
+  </si>
+  <si>
+    <t>5. Click Accept</t>
+  </si>
+  <si>
+    <t>6. Main Calendar screen displays new calendar</t>
+  </si>
+  <si>
+    <t>Verify user can accept changes made by AS</t>
+  </si>
+  <si>
+    <t>Auto.Diff.Reject</t>
+  </si>
+  <si>
+    <t>6. Main Calendar screen displays previous calendar</t>
+  </si>
+  <si>
+    <t>Verify user can reject changes made by AS and keep their previous calendar</t>
+  </si>
+  <si>
+    <t>User can accept calendar generated by AS. Their main schedule is now the version generated by the AS.</t>
+  </si>
+  <si>
+    <t>User can reject calendar generated by AS. Their main schedule remains unchanged.</t>
+  </si>
+  <si>
+    <t>T_Diff_3</t>
+  </si>
+  <si>
+    <t>Auto.Diff.Edit</t>
+  </si>
+  <si>
+    <t>Verify user can input changes to schedule generated by AS.</t>
+  </si>
+  <si>
+    <t>User can input changes to the  calendar generated by AS.</t>
+  </si>
+  <si>
+    <t>5. Click Reject</t>
+  </si>
+  <si>
+    <t>5. Click on event and change parameters</t>
+  </si>
+  <si>
+    <t>6. Event appears on the calendar with new parameters</t>
   </si>
 </sst>
 </file>
@@ -269,7 +362,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="5">
+  <cellXfs count="6">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
@@ -278,6 +371,9 @@
       <alignment horizontal="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
@@ -563,10 +659,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:I41"/>
+  <dimension ref="A1:I68"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A24" workbookViewId="0">
-      <selection activeCell="D40" sqref="D40"/>
+    <sheetView tabSelected="1" topLeftCell="A59" workbookViewId="0">
+      <selection activeCell="E63" sqref="E63:E68"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -654,10 +750,10 @@
       </c>
       <c r="E4" s="4"/>
       <c r="H4" s="2" t="s">
-        <v>40</v>
+        <v>42</v>
       </c>
       <c r="I4" s="2" t="s">
-        <v>41</v>
+        <v>43</v>
       </c>
     </row>
     <row r="5" spans="1:9" ht="30" x14ac:dyDescent="0.25">
@@ -867,7 +963,7 @@
       <c r="B23" s="4"/>
       <c r="C23" s="4"/>
       <c r="D23" s="2" t="s">
-        <v>56</v>
+        <v>58</v>
       </c>
       <c r="E23" s="4"/>
     </row>
@@ -891,19 +987,19 @@
     </row>
     <row r="26" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A26" s="4" t="s">
-        <v>43</v>
+        <v>45</v>
       </c>
       <c r="B26" s="4" t="s">
-        <v>39</v>
+        <v>41</v>
       </c>
       <c r="C26" s="4" t="s">
-        <v>47</v>
+        <v>49</v>
       </c>
       <c r="D26" s="2" t="s">
         <v>14</v>
       </c>
       <c r="E26" s="4" t="s">
-        <v>42</v>
+        <v>44</v>
       </c>
     </row>
     <row r="27" spans="1:5" x14ac:dyDescent="0.25">
@@ -911,7 +1007,7 @@
       <c r="B27" s="4"/>
       <c r="C27" s="4"/>
       <c r="D27" s="2" t="s">
-        <v>44</v>
+        <v>46</v>
       </c>
       <c r="E27" s="4"/>
     </row>
@@ -935,19 +1031,19 @@
     </row>
     <row r="30" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A30" s="4" t="s">
-        <v>45</v>
+        <v>47</v>
       </c>
       <c r="B30" s="4" t="s">
-        <v>46</v>
+        <v>48</v>
       </c>
       <c r="C30" s="4" t="s">
-        <v>50</v>
+        <v>52</v>
       </c>
       <c r="D30" s="2" t="s">
         <v>14</v>
       </c>
       <c r="E30" s="4" t="s">
-        <v>49</v>
+        <v>51</v>
       </c>
     </row>
     <row r="31" spans="1:5" x14ac:dyDescent="0.25">
@@ -955,7 +1051,7 @@
       <c r="B31" s="4"/>
       <c r="C31" s="4"/>
       <c r="D31" s="2" t="s">
-        <v>48</v>
+        <v>50</v>
       </c>
       <c r="E31" s="4"/>
     </row>
@@ -979,19 +1075,19 @@
     </row>
     <row r="34" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A34" s="4" t="s">
-        <v>51</v>
+        <v>53</v>
       </c>
       <c r="B34" s="4" t="s">
-        <v>52</v>
+        <v>54</v>
       </c>
       <c r="C34" s="4" t="s">
-        <v>53</v>
+        <v>55</v>
       </c>
       <c r="D34" s="2" t="s">
-        <v>55</v>
+        <v>57</v>
       </c>
       <c r="E34" s="4" t="s">
-        <v>57</v>
+        <v>59</v>
       </c>
     </row>
     <row r="35" spans="1:5" ht="30" x14ac:dyDescent="0.25">
@@ -999,7 +1095,7 @@
       <c r="B35" s="4"/>
       <c r="C35" s="4"/>
       <c r="D35" s="2" t="s">
-        <v>54</v>
+        <v>56</v>
       </c>
       <c r="E35" s="4"/>
     </row>
@@ -1023,19 +1119,19 @@
     </row>
     <row r="38" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A38" s="4" t="s">
-        <v>51</v>
+        <v>64</v>
       </c>
       <c r="B38" s="4" t="s">
-        <v>58</v>
+        <v>60</v>
       </c>
       <c r="C38" s="4" t="s">
-        <v>59</v>
+        <v>61</v>
       </c>
       <c r="D38" s="2" t="s">
         <v>14</v>
       </c>
       <c r="E38" s="4" t="s">
-        <v>60</v>
+        <v>62</v>
       </c>
     </row>
     <row r="39" spans="1:5" ht="90" x14ac:dyDescent="0.25">
@@ -1043,7 +1139,7 @@
       <c r="B39" s="4"/>
       <c r="C39" s="4"/>
       <c r="D39" s="2" t="s">
-        <v>61</v>
+        <v>63</v>
       </c>
       <c r="E39" s="4"/>
     </row>
@@ -1065,8 +1161,305 @@
       </c>
       <c r="E41" s="4"/>
     </row>
+    <row r="42" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A42" s="4" t="s">
+        <v>67</v>
+      </c>
+      <c r="B42" s="5" t="s">
+        <v>66</v>
+      </c>
+      <c r="C42" s="4" t="s">
+        <v>61</v>
+      </c>
+      <c r="D42" s="2" t="s">
+        <v>14</v>
+      </c>
+      <c r="E42" s="4" t="s">
+        <v>68</v>
+      </c>
+    </row>
+    <row r="43" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A43" s="4"/>
+      <c r="B43" s="5" t="s">
+        <v>39</v>
+      </c>
+      <c r="C43" s="4"/>
+      <c r="D43" s="2" t="s">
+        <v>46</v>
+      </c>
+      <c r="E43" s="4"/>
+    </row>
+    <row r="44" spans="1:5" ht="30" x14ac:dyDescent="0.25">
+      <c r="A44" s="4"/>
+      <c r="B44" s="5" t="s">
+        <v>40</v>
+      </c>
+      <c r="C44" s="4"/>
+      <c r="D44" s="2" t="s">
+        <v>16</v>
+      </c>
+      <c r="E44" s="4"/>
+    </row>
+    <row r="45" spans="1:5" ht="30" x14ac:dyDescent="0.25">
+      <c r="A45" s="4"/>
+      <c r="B45" s="5"/>
+      <c r="C45" s="4"/>
+      <c r="D45" s="2" t="s">
+        <v>17</v>
+      </c>
+      <c r="E45" s="4"/>
+    </row>
+    <row r="47" spans="1:5" ht="45" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A47" s="4" t="s">
+        <v>69</v>
+      </c>
+      <c r="B47" s="4" t="s">
+        <v>65</v>
+      </c>
+      <c r="C47" s="4" t="s">
+        <v>70</v>
+      </c>
+      <c r="D47" s="2" t="s">
+        <v>71</v>
+      </c>
+      <c r="E47" s="4" t="s">
+        <v>75</v>
+      </c>
+    </row>
+    <row r="48" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A48" s="4"/>
+      <c r="B48" s="4"/>
+      <c r="C48" s="4"/>
+      <c r="D48" s="2" t="s">
+        <v>72</v>
+      </c>
+      <c r="E48" s="4"/>
+    </row>
+    <row r="49" spans="1:5" ht="30" x14ac:dyDescent="0.25">
+      <c r="A49" s="4"/>
+      <c r="B49" s="4"/>
+      <c r="C49" s="4"/>
+      <c r="D49" s="2" t="s">
+        <v>73</v>
+      </c>
+      <c r="E49" s="4"/>
+    </row>
+    <row r="50" spans="1:5" ht="45" x14ac:dyDescent="0.25">
+      <c r="A50" s="4"/>
+      <c r="B50" s="4"/>
+      <c r="C50" s="4"/>
+      <c r="D50" s="2" t="s">
+        <v>74</v>
+      </c>
+      <c r="E50" s="4"/>
+    </row>
+    <row r="51" spans="1:5" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A51" s="4" t="s">
+        <v>76</v>
+      </c>
+      <c r="B51" s="4" t="s">
+        <v>77</v>
+      </c>
+      <c r="C51" s="4" t="s">
+        <v>80</v>
+      </c>
+      <c r="D51" s="2" t="s">
+        <v>71</v>
+      </c>
+      <c r="E51" s="4" t="s">
+        <v>84</v>
+      </c>
+    </row>
+    <row r="52" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A52" s="4"/>
+      <c r="B52" s="4"/>
+      <c r="C52" s="4"/>
+      <c r="D52" s="2" t="s">
+        <v>72</v>
+      </c>
+      <c r="E52" s="4"/>
+    </row>
+    <row r="53" spans="1:5" ht="30" x14ac:dyDescent="0.25">
+      <c r="A53" s="4"/>
+      <c r="B53" s="4"/>
+      <c r="C53" s="4"/>
+      <c r="D53" s="2" t="s">
+        <v>73</v>
+      </c>
+      <c r="E53" s="4"/>
+    </row>
+    <row r="54" spans="1:5" ht="45" x14ac:dyDescent="0.25">
+      <c r="A54" s="4"/>
+      <c r="B54" s="4"/>
+      <c r="C54" s="4"/>
+      <c r="D54" s="2" t="s">
+        <v>74</v>
+      </c>
+      <c r="E54" s="4"/>
+    </row>
+    <row r="55" spans="1:5" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A55" s="4"/>
+      <c r="B55" s="4"/>
+      <c r="C55" s="4"/>
+      <c r="D55" s="2" t="s">
+        <v>78</v>
+      </c>
+      <c r="E55" s="4"/>
+    </row>
+    <row r="56" spans="1:5" ht="30" x14ac:dyDescent="0.25">
+      <c r="A56" s="4"/>
+      <c r="B56" s="4"/>
+      <c r="C56" s="4"/>
+      <c r="D56" s="2" t="s">
+        <v>79</v>
+      </c>
+      <c r="E56" s="4"/>
+    </row>
+    <row r="57" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A57" s="4" t="s">
+        <v>86</v>
+      </c>
+      <c r="B57" s="4" t="s">
+        <v>81</v>
+      </c>
+      <c r="C57" s="4" t="s">
+        <v>83</v>
+      </c>
+      <c r="D57" s="2" t="s">
+        <v>71</v>
+      </c>
+      <c r="E57" s="4" t="s">
+        <v>85</v>
+      </c>
+    </row>
+    <row r="58" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A58" s="4"/>
+      <c r="B58" s="4"/>
+      <c r="C58" s="4"/>
+      <c r="D58" s="2" t="s">
+        <v>72</v>
+      </c>
+      <c r="E58" s="4"/>
+    </row>
+    <row r="59" spans="1:5" ht="30" x14ac:dyDescent="0.25">
+      <c r="A59" s="4"/>
+      <c r="B59" s="4"/>
+      <c r="C59" s="4"/>
+      <c r="D59" s="2" t="s">
+        <v>73</v>
+      </c>
+      <c r="E59" s="4"/>
+    </row>
+    <row r="60" spans="1:5" ht="45" x14ac:dyDescent="0.25">
+      <c r="A60" s="4"/>
+      <c r="B60" s="4"/>
+      <c r="C60" s="4"/>
+      <c r="D60" s="2" t="s">
+        <v>74</v>
+      </c>
+      <c r="E60" s="4"/>
+    </row>
+    <row r="61" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A61" s="4"/>
+      <c r="B61" s="4"/>
+      <c r="C61" s="4"/>
+      <c r="D61" s="2" t="s">
+        <v>90</v>
+      </c>
+      <c r="E61" s="4"/>
+    </row>
+    <row r="62" spans="1:5" ht="30" x14ac:dyDescent="0.25">
+      <c r="A62" s="4"/>
+      <c r="B62" s="4"/>
+      <c r="C62" s="4"/>
+      <c r="D62" s="2" t="s">
+        <v>82</v>
+      </c>
+      <c r="E62" s="4"/>
+    </row>
+    <row r="63" spans="1:5" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A63" s="4" t="s">
+        <v>86</v>
+      </c>
+      <c r="B63" s="4" t="s">
+        <v>87</v>
+      </c>
+      <c r="C63" s="4" t="s">
+        <v>88</v>
+      </c>
+      <c r="D63" s="2" t="s">
+        <v>71</v>
+      </c>
+      <c r="E63" s="4" t="s">
+        <v>89</v>
+      </c>
+    </row>
+    <row r="64" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A64" s="4"/>
+      <c r="B64" s="4"/>
+      <c r="C64" s="4"/>
+      <c r="D64" s="2" t="s">
+        <v>72</v>
+      </c>
+      <c r="E64" s="4"/>
+    </row>
+    <row r="65" spans="1:5" ht="30" x14ac:dyDescent="0.25">
+      <c r="A65" s="4"/>
+      <c r="B65" s="4"/>
+      <c r="C65" s="4"/>
+      <c r="D65" s="2" t="s">
+        <v>73</v>
+      </c>
+      <c r="E65" s="4"/>
+    </row>
+    <row r="66" spans="1:5" ht="45" x14ac:dyDescent="0.25">
+      <c r="A66" s="4"/>
+      <c r="B66" s="4"/>
+      <c r="C66" s="4"/>
+      <c r="D66" s="2" t="s">
+        <v>74</v>
+      </c>
+      <c r="E66" s="4"/>
+    </row>
+    <row r="67" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A67" s="4"/>
+      <c r="B67" s="4"/>
+      <c r="C67" s="4"/>
+      <c r="D67" s="2" t="s">
+        <v>91</v>
+      </c>
+      <c r="E67" s="4"/>
+    </row>
+    <row r="68" spans="1:5" ht="30" x14ac:dyDescent="0.25">
+      <c r="A68" s="4"/>
+      <c r="B68" s="4"/>
+      <c r="C68" s="4"/>
+      <c r="D68" s="2" t="s">
+        <v>92</v>
+      </c>
+      <c r="E68" s="4"/>
+    </row>
   </sheetData>
-  <mergeCells count="40">
+  <mergeCells count="59">
+    <mergeCell ref="A63:A68"/>
+    <mergeCell ref="B63:B68"/>
+    <mergeCell ref="C63:C68"/>
+    <mergeCell ref="E63:E68"/>
+    <mergeCell ref="C51:C56"/>
+    <mergeCell ref="E51:E56"/>
+    <mergeCell ref="A57:A62"/>
+    <mergeCell ref="B57:B62"/>
+    <mergeCell ref="C57:C62"/>
+    <mergeCell ref="E57:E62"/>
+    <mergeCell ref="A51:A56"/>
+    <mergeCell ref="B51:B56"/>
+    <mergeCell ref="A42:A45"/>
+    <mergeCell ref="C42:C45"/>
+    <mergeCell ref="E42:E45"/>
+    <mergeCell ref="A47:A50"/>
+    <mergeCell ref="B47:B50"/>
+    <mergeCell ref="C47:C50"/>
+    <mergeCell ref="E47:E50"/>
     <mergeCell ref="A34:A37"/>
     <mergeCell ref="B34:B37"/>
     <mergeCell ref="C34:C37"/>

</xml_diff>

<commit_message>
added two brief tests for deadline event creation
</commit_message>
<xml_diff>
--- a/FuncTestPlanAutoScheduler.xlsx
+++ b/FuncTestPlanAutoScheduler.xlsx
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="141" uniqueCount="93">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="157" uniqueCount="103">
   <si>
     <t>Test ID</t>
   </si>
@@ -303,6 +303,36 @@
   </si>
   <si>
     <t>6. Event appears on the calendar with new parameters</t>
+  </si>
+  <si>
+    <t>T_Dead_1</t>
+  </si>
+  <si>
+    <t>Event.Deadline.Deadline</t>
+  </si>
+  <si>
+    <t>Verify user can create a deadline event with a deadline member.</t>
+  </si>
+  <si>
+    <t>4. Verify the that the Deadline event object was created with the correct deadline member</t>
+  </si>
+  <si>
+    <t>Deadline object is created with user given deadline member.</t>
+  </si>
+  <si>
+    <t>T_Dead_2</t>
+  </si>
+  <si>
+    <t>Event.Deadline.WorkTime</t>
+  </si>
+  <si>
+    <t>Verify user can create a deadline event with a work time member.</t>
+  </si>
+  <si>
+    <t>4. Verify the that the Deadline event object was created with the correct work time member</t>
+  </si>
+  <si>
+    <t>Deadline object is created with user given work time member.</t>
   </si>
 </sst>
 </file>
@@ -659,10 +689,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:I68"/>
+  <dimension ref="A1:I77"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A59" workbookViewId="0">
-      <selection activeCell="E63" sqref="E63:E68"/>
+    <sheetView tabSelected="1" topLeftCell="A61" workbookViewId="0">
+      <selection activeCell="C74" sqref="C74:C77"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1439,8 +1469,104 @@
       </c>
       <c r="E68" s="4"/>
     </row>
+    <row r="70" spans="1:5" ht="30" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A70" s="4" t="s">
+        <v>93</v>
+      </c>
+      <c r="B70" s="4" t="s">
+        <v>94</v>
+      </c>
+      <c r="C70" s="4" t="s">
+        <v>95</v>
+      </c>
+      <c r="D70" s="2" t="s">
+        <v>71</v>
+      </c>
+      <c r="E70" s="4" t="s">
+        <v>97</v>
+      </c>
+    </row>
+    <row r="71" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A71" s="4"/>
+      <c r="B71" s="4"/>
+      <c r="C71" s="4"/>
+      <c r="D71" s="2" t="s">
+        <v>72</v>
+      </c>
+      <c r="E71" s="4"/>
+    </row>
+    <row r="72" spans="1:5" ht="30" x14ac:dyDescent="0.25">
+      <c r="A72" s="4"/>
+      <c r="B72" s="4"/>
+      <c r="C72" s="4"/>
+      <c r="D72" s="2" t="s">
+        <v>73</v>
+      </c>
+      <c r="E72" s="4"/>
+    </row>
+    <row r="73" spans="1:5" ht="45" x14ac:dyDescent="0.25">
+      <c r="A73" s="4"/>
+      <c r="B73" s="4"/>
+      <c r="C73" s="4"/>
+      <c r="D73" s="2" t="s">
+        <v>96</v>
+      </c>
+      <c r="E73" s="4"/>
+    </row>
+    <row r="74" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A74" s="4" t="s">
+        <v>98</v>
+      </c>
+      <c r="B74" s="4" t="s">
+        <v>99</v>
+      </c>
+      <c r="C74" s="4" t="s">
+        <v>100</v>
+      </c>
+      <c r="D74" s="2" t="s">
+        <v>71</v>
+      </c>
+      <c r="E74" s="4" t="s">
+        <v>102</v>
+      </c>
+    </row>
+    <row r="75" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A75" s="4"/>
+      <c r="B75" s="4"/>
+      <c r="C75" s="4"/>
+      <c r="D75" s="2" t="s">
+        <v>72</v>
+      </c>
+      <c r="E75" s="4"/>
+    </row>
+    <row r="76" spans="1:5" ht="30" x14ac:dyDescent="0.25">
+      <c r="A76" s="4"/>
+      <c r="B76" s="4"/>
+      <c r="C76" s="4"/>
+      <c r="D76" s="2" t="s">
+        <v>73</v>
+      </c>
+      <c r="E76" s="4"/>
+    </row>
+    <row r="77" spans="1:5" ht="45" x14ac:dyDescent="0.25">
+      <c r="A77" s="4"/>
+      <c r="B77" s="4"/>
+      <c r="C77" s="4"/>
+      <c r="D77" s="2" t="s">
+        <v>101</v>
+      </c>
+      <c r="E77" s="4"/>
+    </row>
   </sheetData>
-  <mergeCells count="59">
+  <mergeCells count="67">
+    <mergeCell ref="A70:A73"/>
+    <mergeCell ref="B70:B73"/>
+    <mergeCell ref="C70:C73"/>
+    <mergeCell ref="E70:E73"/>
+    <mergeCell ref="A74:A77"/>
+    <mergeCell ref="B74:B77"/>
+    <mergeCell ref="C74:C77"/>
+    <mergeCell ref="E74:E77"/>
     <mergeCell ref="A63:A68"/>
     <mergeCell ref="B63:B68"/>
     <mergeCell ref="C63:C68"/>

</xml_diff>